<commit_message>
Lavoro su data procedure invasive
</commit_message>
<xml_diff>
--- a/data/Tabella procedure invasive.xlsx
+++ b/data/Tabella procedure invasive.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariagraziacicala/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariagraziacicala/Desktop/ica_cost2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E9053AB-3346-0C44-88C8-DF90C7BDAD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E355DC67-B71E-0740-B6B6-1E45A4C0A1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="500" windowWidth="21300" windowHeight="15720" xr2:uid="{5739CAE7-9D7F-CF46-B86B-E63FDA5D688A}"/>
+    <workbookView xWindow="11040" yWindow="660" windowWidth="21300" windowHeight="15720" xr2:uid="{5739CAE7-9D7F-CF46-B86B-E63FDA5D688A}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>Interventi Chirurgici e Procedure invasive (ICD9-CM)</t>
   </si>
@@ -102,6 +102,21 @@
   </si>
   <si>
     <t>Colonna1</t>
+  </si>
+  <si>
+    <t>Respiratorio</t>
+  </si>
+  <si>
+    <t>Colonna2</t>
+  </si>
+  <si>
+    <t>Sangue</t>
+  </si>
+  <si>
+    <t>Urinario</t>
+  </si>
+  <si>
+    <t>Ferita</t>
   </si>
 </sst>
 </file>
@@ -200,11 +215,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{06D85F5E-46EB-C646-BA16-921A35E1975E}" name="Tabella1" displayName="Tabella1" ref="A1:B20" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:B20" xr:uid="{06D85F5E-46EB-C646-BA16-921A35E1975E}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{06D85F5E-46EB-C646-BA16-921A35E1975E}" name="Tabella1" displayName="Tabella1" ref="A1:C20" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C20" xr:uid="{06D85F5E-46EB-C646-BA16-921A35E1975E}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{4D282D1C-C140-2A45-9195-EF4EB037BDAD}" name="Interventi Chirurgici e Procedure invasive (ICD9-CM)"/>
     <tableColumn id="2" xr3:uid="{2B5FFA1F-7A2D-7741-A111-9508FD507D42}" name="Colonna1"/>
+    <tableColumn id="3" xr3:uid="{3FC68C2B-5229-1B4C-9DBD-CF0FDF0B31AC}" name="Colonna2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -507,27 +523,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC030296-BD9C-D849-89B2-94DD1DF7D3AB}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="2" max="2" width="60.33203125" customWidth="1"/>
+    <col min="2" max="2" width="61.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -535,148 +554,202 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>311</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3129</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3891</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3893</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3894</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3895</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>598</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>5794</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8607</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8622</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>8628</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>8962</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>8964</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>9604</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>9605</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>9670</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>9671</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>9672</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>